<commit_message>
Added Object Locators for Login Page and a working testcase
</commit_message>
<xml_diff>
--- a/src/test/resources/objectLocators/ObjectLocators.xlsx
+++ b/src/test/resources/objectLocators/ObjectLocators.xlsx
@@ -1,13 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5B0EA7-2A3E-4E8F-8ABF-8D8BF0C176F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="6492" yWindow="828" windowWidth="14460" windowHeight="6732" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
+    <sheet name="Locators" sheetId="2" r:id="rId2"/>
+    <sheet name="Validators" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,8 +21,55 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+  <si>
+    <t>userNameBox</t>
+  </si>
+  <si>
+    <t>passwordBox</t>
+  </si>
+  <si>
+    <t>LoginButton</t>
+  </si>
+  <si>
+    <t>XPATH</t>
+  </si>
+  <si>
+    <t>LOCATORS</t>
+  </si>
+  <si>
+    <t>CSS</t>
+  </si>
+  <si>
+    <t>CLASSNAME</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>LINK</t>
+  </si>
+  <si>
+    <t>PARTIALLINK</t>
+  </si>
+  <si>
+    <t>//input[@name='username']</t>
+  </si>
+  <si>
+    <t>//input[@name='password']</t>
+  </si>
+  <si>
+    <t>//button[@type='submit']</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -37,7 +87,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -45,12 +95,180 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,12 +548,138 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DE25883-DCC9-4F85-9BA8-2F4A6EC349D2}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB348F02-31C0-45FD-9936-2F34A8ACAD78}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added dashboard page and xpath for the same
</commit_message>
<xml_diff>
--- a/src/test/resources/objectLocators/ObjectLocators.xlsx
+++ b/src/test/resources/objectLocators/ObjectLocators.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5B0EA7-2A3E-4E8F-8ABF-8D8BF0C176F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3CB2F6-5E58-4E59-B200-5AFD115B6378}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6492" yWindow="828" windowWidth="14460" windowHeight="6732" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6492" yWindow="828" windowWidth="14460" windowHeight="6732" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
-    <sheet name="Locators" sheetId="2" r:id="rId2"/>
-    <sheet name="Validators" sheetId="3" r:id="rId3"/>
+    <sheet name="DashboardPage" sheetId="4" r:id="rId2"/>
+    <sheet name="Locators" sheetId="2" r:id="rId3"/>
+    <sheet name="Validators" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>userNameBox</t>
   </si>
@@ -64,6 +65,12 @@
   </si>
   <si>
     <t>//button[@type='submit']</t>
+  </si>
+  <si>
+    <t>//h6[@class='oxd-text oxd-text--h6 oxd-topbar-header-breadcrumb-module']</t>
+  </si>
+  <si>
+    <t>DashboardPageLogo</t>
   </si>
 </sst>
 </file>
@@ -551,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -600,6 +607,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F49DF72-72ED-4C8E-AB0A-6DEED788B86A}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="65.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DE25883-DCC9-4F85-9BA8-2F4A6EC349D2}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -673,7 +710,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB348F02-31C0-45FD-9936-2F34A8ACAD78}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added extent reports properties
</commit_message>
<xml_diff>
--- a/src/test/resources/objectLocators/ObjectLocators.xlsx
+++ b/src/test/resources/objectLocators/ObjectLocators.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3CB2F6-5E58-4E59-B200-5AFD115B6378}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD953CD-3BA7-42F0-BCC6-45993141D93B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6492" yWindow="828" windowWidth="14460" windowHeight="6732" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6492" yWindow="828" windowWidth="14460" windowHeight="6732" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>userNameBox</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>DashboardPageLogo</t>
+  </si>
+  <si>
+    <t>//p[@class='oxd-text oxd-text--p oxd-alert-content-text']</t>
+  </si>
+  <si>
+    <t>invalidCredentialsMessage</t>
   </si>
 </sst>
 </file>
@@ -556,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -601,6 +607,17 @@
         <v>13</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -610,7 +627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F49DF72-72ED-4C8E-AB0A-6DEED788B86A}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added working testcase for add employee including autoIt
</commit_message>
<xml_diff>
--- a/src/test/resources/objectLocators/ObjectLocators.xlsx
+++ b/src/test/resources/objectLocators/ObjectLocators.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD953CD-3BA7-42F0-BCC6-45993141D93B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FCB5DB-3AD1-4D8B-80F9-1D070C23A4C6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6492" yWindow="828" windowWidth="14460" windowHeight="6732" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7188" yWindow="2088" windowWidth="14460" windowHeight="6732" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
     <sheet name="DashboardPage" sheetId="4" r:id="rId2"/>
-    <sheet name="Locators" sheetId="2" r:id="rId3"/>
-    <sheet name="Validators" sheetId="3" r:id="rId4"/>
+    <sheet name="PIMPage" sheetId="5" r:id="rId3"/>
+    <sheet name="Locators" sheetId="2" r:id="rId4"/>
+    <sheet name="Validators" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>userNameBox</t>
   </si>
@@ -77,6 +78,72 @@
   </si>
   <si>
     <t>invalidCredentialsMessage</t>
+  </si>
+  <si>
+    <t>addEmployeeNavigationMenuButton</t>
+  </si>
+  <si>
+    <t>firstNameTextBox</t>
+  </si>
+  <si>
+    <t>middleNameTextBox</t>
+  </si>
+  <si>
+    <t>lastNameTextBox</t>
+  </si>
+  <si>
+    <t>employeeIdTextBox</t>
+  </si>
+  <si>
+    <t>loginDetailsToggle</t>
+  </si>
+  <si>
+    <t>setUsernameTextBox</t>
+  </si>
+  <si>
+    <t>setPasswordTextBox</t>
+  </si>
+  <si>
+    <t>confirmPasswordTextBox</t>
+  </si>
+  <si>
+    <t>//a[@class='oxd-topbar-body-nav-tab-item' and text()='Add Employee']</t>
+  </si>
+  <si>
+    <t>//input[@name='firstName']</t>
+  </si>
+  <si>
+    <t>//input[@name='middleName']</t>
+  </si>
+  <si>
+    <t>//input[@name='lastName']</t>
+  </si>
+  <si>
+    <t>(//input[@class='oxd-input oxd-input--active'])[2]</t>
+  </si>
+  <si>
+    <t>(//div[@class='oxd-input-group oxd-input-field-bottom-space']/div/input[@class='oxd-input oxd-input--active'])[2]</t>
+  </si>
+  <si>
+    <t>(//input[@type='password'])[1]</t>
+  </si>
+  <si>
+    <t>(//input[@type='password'])[2]</t>
+  </si>
+  <si>
+    <t>pimDashboardLocator</t>
+  </si>
+  <si>
+    <t>//span[@class='oxd-text oxd-text--span oxd-main-menu-item--name' and text()='PIM']</t>
+  </si>
+  <si>
+    <t>//div[@class='oxd-switch-wrapper']/label</t>
+  </si>
+  <si>
+    <t>uploadProfilePictureButton</t>
+  </si>
+  <si>
+    <t>//button[@class='oxd-icon-button employee-image-action']</t>
   </si>
 </sst>
 </file>
@@ -564,7 +631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -625,15 +692,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F49DF72-72ED-4C8E-AB0A-6DEED788B86A}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
     <col min="3" max="3" width="65.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -648,12 +715,152 @@
         <v>14</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF9EBE50-FCC2-4A84-B3D4-1EBBC41843F2}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="38.21875" customWidth="1"/>
+    <col min="3" max="3" width="62" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DE25883-DCC9-4F85-9BA8-2F4A6EC349D2}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -727,7 +934,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB348F02-31C0-45FD-9936-2F34A8ACAD78}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Completed Testcase to add employee
</commit_message>
<xml_diff>
--- a/src/test/resources/objectLocators/ObjectLocators.xlsx
+++ b/src/test/resources/objectLocators/ObjectLocators.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FCB5DB-3AD1-4D8B-80F9-1D070C23A4C6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C42FBB7-15AA-47FF-9855-8230D6AF0C40}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7188" yWindow="2088" windowWidth="14460" windowHeight="6732" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
   <si>
     <t>userNameBox</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>//button[@class='oxd-icon-button employee-image-action']</t>
+  </si>
+  <si>
+    <t>saveEmployeeButton</t>
   </si>
 </sst>
 </file>
@@ -733,10 +736,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF9EBE50-FCC2-4A84-B3D4-1EBBC41843F2}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -853,6 +856,17 @@
       </c>
       <c r="C10" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Object Locators for Search Employee Scenario
</commit_message>
<xml_diff>
--- a/src/test/resources/objectLocators/ObjectLocators.xlsx
+++ b/src/test/resources/objectLocators/ObjectLocators.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C42FBB7-15AA-47FF-9855-8230D6AF0C40}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BA8913-F77B-4B14-A59B-2603E6490A7E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7188" yWindow="2088" windowWidth="14460" windowHeight="6732" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
   <si>
     <t>userNameBox</t>
   </si>
@@ -119,9 +119,6 @@
     <t>//input[@name='lastName']</t>
   </si>
   <si>
-    <t>(//input[@class='oxd-input oxd-input--active'])[2]</t>
-  </si>
-  <si>
     <t>(//div[@class='oxd-input-group oxd-input-field-bottom-space']/div/input[@class='oxd-input oxd-input--active'])[2]</t>
   </si>
   <si>
@@ -147,6 +144,45 @@
   </si>
   <si>
     <t>saveEmployeeButton</t>
+  </si>
+  <si>
+    <t>//label[text()='Employee Id']/parent::div/following-sibling::div/input</t>
+  </si>
+  <si>
+    <t>searchEmployeeNameField</t>
+  </si>
+  <si>
+    <t>searchEmployeeButtonLocator</t>
+  </si>
+  <si>
+    <t>searchedEmployeeIdRecordTable</t>
+  </si>
+  <si>
+    <t>profileNameLocator</t>
+  </si>
+  <si>
+    <t>//label[text()='Employee Name']/parent::div/following-sibling::div/div/div/input</t>
+  </si>
+  <si>
+    <t>//button[text()=' Search ']</t>
+  </si>
+  <si>
+    <t>searchedEmployeeFirstNameRecordTable</t>
+  </si>
+  <si>
+    <t>searchedEmployeeLastNameRecordTable</t>
+  </si>
+  <si>
+    <t>(//div[@class='oxd-table-cell oxd-padding-cell']/div)[3]</t>
+  </si>
+  <si>
+    <t>(//div[@class='oxd-table-cell oxd-padding-cell']/div)[4]</t>
+  </si>
+  <si>
+    <t>(//div[@class='oxd-table-cell oxd-padding-cell']/div)[2]</t>
+  </si>
+  <si>
+    <t>//p[@class='oxd-userdropdown-name']</t>
   </si>
 </sst>
 </file>
@@ -695,10 +731,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F49DF72-72ED-4C8E-AB0A-6DEED788B86A}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -720,13 +756,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>36</v>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -736,16 +783,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF9EBE50-FCC2-4A84-B3D4-1EBBC41843F2}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="38.21875" customWidth="1"/>
-    <col min="3" max="3" width="62" customWidth="1"/>
+    <col min="3" max="3" width="68.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -800,7 +847,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -811,7 +858,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -822,7 +869,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -833,7 +880,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -844,29 +891,84 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
         <v>38</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Locators for GlobalsqaDemoSite
</commit_message>
<xml_diff>
--- a/src/test/resources/objectLocators/ObjectLocators.xlsx
+++ b/src/test/resources/objectLocators/ObjectLocators.xlsx
@@ -3,16 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BA8913-F77B-4B14-A59B-2603E6490A7E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495E1378-E4C2-4D7B-8B07-B61FB0456D83}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
     <sheet name="DashboardPage" sheetId="4" r:id="rId2"/>
-    <sheet name="PIMPage" sheetId="5" r:id="rId3"/>
-    <sheet name="Locators" sheetId="2" r:id="rId4"/>
-    <sheet name="Validators" sheetId="3" r:id="rId5"/>
+    <sheet name="GlobalsqaDemoSite" sheetId="6" r:id="rId3"/>
+    <sheet name="PIMPage" sheetId="5" r:id="rId4"/>
+    <sheet name="Locators" sheetId="2" r:id="rId5"/>
+    <sheet name="Validators" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="63">
   <si>
     <t>userNameBox</t>
   </si>
@@ -183,6 +184,36 @@
   </si>
   <si>
     <t>//p[@class='oxd-userdropdown-name']</t>
+  </si>
+  <si>
+    <t>dragAndDropButton</t>
+  </si>
+  <si>
+    <t>sourceImageLocator</t>
+  </si>
+  <si>
+    <t>destiantionTrashLocator</t>
+  </si>
+  <si>
+    <t>//a[text()='DragAndDrop']</t>
+  </si>
+  <si>
+    <t>closeAdPopUpLocator</t>
+  </si>
+  <si>
+    <t>//span[text()='Close']</t>
+  </si>
+  <si>
+    <t>//div[@id='trash']</t>
+  </si>
+  <si>
+    <t>frameLocator</t>
+  </si>
+  <si>
+    <t>//iframe[@class='demo-frame lazyloaded']</t>
+  </si>
+  <si>
+    <t>//h5[text()='High Tatras']/parent::li</t>
   </si>
 </sst>
 </file>
@@ -733,7 +764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F49DF72-72ED-4C8E-AB0A-6DEED788B86A}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -782,6 +813,80 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5278E5E8-F516-428C-92F2-3F489AA4F744}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.5546875" customWidth="1"/>
+    <col min="3" max="3" width="44.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF9EBE50-FCC2-4A84-B3D4-1EBBC41843F2}">
   <dimension ref="A1:C16"/>
   <sheetViews>
@@ -976,7 +1081,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DE25883-DCC9-4F85-9BA8-2F4A6EC349D2}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -1050,7 +1155,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB348F02-31C0-45FD-9936-2F34A8ACAD78}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added object locators for jira testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/objectLocators/ObjectLocators.xlsx
+++ b/src/test/resources/objectLocators/ObjectLocators.xlsx
@@ -3,17 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495E1378-E4C2-4D7B-8B07-B61FB0456D83}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3505C924-BD72-433D-AC23-803030FD899E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
     <sheet name="DashboardPage" sheetId="4" r:id="rId2"/>
     <sheet name="GlobalsqaDemoSite" sheetId="6" r:id="rId3"/>
     <sheet name="PIMPage" sheetId="5" r:id="rId4"/>
-    <sheet name="Locators" sheetId="2" r:id="rId5"/>
-    <sheet name="Validators" sheetId="3" r:id="rId6"/>
+    <sheet name="Jira" sheetId="7" r:id="rId5"/>
+    <sheet name="Locators" sheetId="2" r:id="rId6"/>
+    <sheet name="Validators" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="88">
   <si>
     <t>userNameBox</t>
   </si>
@@ -214,6 +215,81 @@
   </si>
   <si>
     <t>//h5[text()='High Tatras']/parent::li</t>
+  </si>
+  <si>
+    <t>jiraLoginEmailLocator</t>
+  </si>
+  <si>
+    <t>jiraLoginContinueButton</t>
+  </si>
+  <si>
+    <t>jiraLoginPasswordLocator</t>
+  </si>
+  <si>
+    <t>jiraLoginButton</t>
+  </si>
+  <si>
+    <t>profileIconLocator</t>
+  </si>
+  <si>
+    <t>nameLocatorInProfile</t>
+  </si>
+  <si>
+    <t>//input[@id='username']</t>
+  </si>
+  <si>
+    <t>//button[@id='login-submit']</t>
+  </si>
+  <si>
+    <t>//input[@id='password']</t>
+  </si>
+  <si>
+    <t>//span[@data-test-id='ak-spotlight-target-profile-spotlight']</t>
+  </si>
+  <si>
+    <t>emailIdLocatorInProfile</t>
+  </si>
+  <si>
+    <t>//div[@class='ohlecc-4 kuteQC']/div[@class='ohlecc-3 cxCHrv']</t>
+  </si>
+  <si>
+    <t>//div[@class='ohlecc-4 kuteQC']/small</t>
+  </si>
+  <si>
+    <t>createButtonLocator</t>
+  </si>
+  <si>
+    <t>summaryBoxLocator</t>
+  </si>
+  <si>
+    <t>descriptionBoxLocator</t>
+  </si>
+  <si>
+    <t>asigneeBoxLocator</t>
+  </si>
+  <si>
+    <t>assignItToMeLocator</t>
+  </si>
+  <si>
+    <t>createButtonLocator2</t>
+  </si>
+  <si>
+    <t>//span[text()='Create']</t>
+  </si>
+  <si>
+    <t>(//span[text()='Create'])[2]</t>
+  </si>
+  <si>
+    <t>//input[@id='summary-field']</t>
+  </si>
+  <si>
+    <t>//div[@class='ua-chrome ProseMirror pm-table-resizing-plugin']</t>
+  </si>
+  <si>
+    <t>(//div[@class='fabric-user-picker__control css-1c1zckh-control'])[1]</t>
+  </si>
+  <si>
+    <t>//span[text()='Assign to me']</t>
   </si>
 </sst>
 </file>
@@ -816,7 +892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5278E5E8-F516-428C-92F2-3F489AA4F744}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -1082,6 +1158,168 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E56147E-86B1-466D-90D0-FA5513DD7E62}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.88671875" customWidth="1"/>
+    <col min="3" max="3" width="62.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DE25883-DCC9-4F85-9BA8-2F4A6EC349D2}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -1155,7 +1393,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB348F02-31C0-45FD-9936-2F34A8ACAD78}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>